<commit_message>
add Pmax calculation adapt Excels for Link
</commit_message>
<xml_diff>
--- a/data/example/Power_Links.xlsx
+++ b/data/example/Power_Links.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\micha\Desktop\GIT\LEGO-Pyomo\data\example\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{941C96A5-DAEE-49B1-9941-B3DC28C05199}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{81DD55D1-2383-46E0-BC61-E50F84394C18}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-98" yWindow="-98" windowWidth="21795" windowHeight="13875" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -114,7 +114,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="74" uniqueCount="41">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="62" uniqueCount="50">
   <si>
     <t>Format:</t>
   </si>
@@ -237,6 +237,33 @@
   </si>
   <si>
     <t>Annualized increase Link power</t>
+  </si>
+  <si>
+    <t>Node_1.1</t>
+  </si>
+  <si>
+    <t>Node_2.1</t>
+  </si>
+  <si>
+    <t>Node_3.1</t>
+  </si>
+  <si>
+    <t>Node_4.1</t>
+  </si>
+  <si>
+    <t>Node_5.1</t>
+  </si>
+  <si>
+    <t>Node_6.1</t>
+  </si>
+  <si>
+    <t>Node_7.1</t>
+  </si>
+  <si>
+    <t>Node_8.1</t>
+  </si>
+  <si>
+    <t>Node_9.1</t>
   </si>
 </sst>
 </file>
@@ -675,13 +702,13 @@
   <sheetPr>
     <tabColor rgb="FF008080"/>
   </sheetPr>
-  <dimension ref="A1:G20"/>
+  <dimension ref="A1:G16"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
       <pane xSplit="2" ySplit="7" topLeftCell="C8" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight"/>
       <selection pane="bottomLeft"/>
-      <selection pane="bottomRight"/>
+      <selection pane="bottomRight" activeCell="I6" sqref="I6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.1328125" defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
@@ -826,7 +853,7 @@
         <v>25</v>
       </c>
       <c r="D8" s="12" t="s">
-        <v>26</v>
+        <v>41</v>
       </c>
       <c r="E8" s="12" t="s">
         <v>27</v>
@@ -845,7 +872,7 @@
         <v>28</v>
       </c>
       <c r="D9" s="12" t="s">
-        <v>29</v>
+        <v>42</v>
       </c>
       <c r="E9" s="12" t="s">
         <v>27</v>
@@ -861,10 +888,10 @@
       <c r="A10" s="10"/>
       <c r="B10" s="11"/>
       <c r="C10" s="12" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="D10" s="12" t="s">
-        <v>26</v>
+        <v>43</v>
       </c>
       <c r="E10" s="12" t="s">
         <v>27</v>
@@ -880,10 +907,10 @@
       <c r="A11" s="10"/>
       <c r="B11" s="11"/>
       <c r="C11" s="12" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="D11" s="12" t="s">
-        <v>30</v>
+        <v>44</v>
       </c>
       <c r="E11" s="12" t="s">
         <v>27</v>
@@ -899,10 +926,10 @@
       <c r="A12" s="10"/>
       <c r="B12" s="11"/>
       <c r="C12" s="12" t="s">
-        <v>29</v>
+        <v>31</v>
       </c>
       <c r="D12" s="12" t="s">
-        <v>26</v>
+        <v>45</v>
       </c>
       <c r="E12" s="12" t="s">
         <v>27</v>
@@ -918,10 +945,10 @@
       <c r="A13" s="10"/>
       <c r="B13" s="11"/>
       <c r="C13" s="12" t="s">
-        <v>30</v>
+        <v>26</v>
       </c>
       <c r="D13" s="12" t="s">
-        <v>31</v>
+        <v>46</v>
       </c>
       <c r="E13" s="12" t="s">
         <v>27</v>
@@ -937,10 +964,10 @@
       <c r="A14" s="10"/>
       <c r="B14" s="11"/>
       <c r="C14" s="12" t="s">
-        <v>30</v>
+        <v>33</v>
       </c>
       <c r="D14" s="12" t="s">
-        <v>26</v>
+        <v>47</v>
       </c>
       <c r="E14" s="12" t="s">
         <v>27</v>
@@ -956,10 +983,10 @@
       <c r="A15" s="10"/>
       <c r="B15" s="11"/>
       <c r="C15" s="12" t="s">
-        <v>30</v>
+        <v>34</v>
       </c>
       <c r="D15" s="12" t="s">
-        <v>32</v>
+        <v>48</v>
       </c>
       <c r="E15" s="12" t="s">
         <v>27</v>
@@ -975,10 +1002,10 @@
       <c r="A16" s="10"/>
       <c r="B16" s="11"/>
       <c r="C16" s="12" t="s">
-        <v>26</v>
+        <v>32</v>
       </c>
       <c r="D16" s="12" t="s">
-        <v>33</v>
+        <v>49</v>
       </c>
       <c r="E16" s="12" t="s">
         <v>27</v>
@@ -987,82 +1014,6 @@
         <v>175</v>
       </c>
       <c r="G16" s="14">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="17" spans="1:7" x14ac:dyDescent="0.45">
-      <c r="A17" s="10"/>
-      <c r="B17" s="11"/>
-      <c r="C17" s="12" t="s">
-        <v>26</v>
-      </c>
-      <c r="D17" s="12" t="s">
-        <v>34</v>
-      </c>
-      <c r="E17" s="12" t="s">
-        <v>27</v>
-      </c>
-      <c r="F17" s="13">
-        <v>175</v>
-      </c>
-      <c r="G17" s="14">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="18" spans="1:7" x14ac:dyDescent="0.45">
-      <c r="A18" s="10"/>
-      <c r="B18" s="11"/>
-      <c r="C18" s="12" t="s">
-        <v>33</v>
-      </c>
-      <c r="D18" s="12" t="s">
-        <v>34</v>
-      </c>
-      <c r="E18" s="12" t="s">
-        <v>27</v>
-      </c>
-      <c r="F18" s="13">
-        <v>175</v>
-      </c>
-      <c r="G18" s="14">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="19" spans="1:7" x14ac:dyDescent="0.45">
-      <c r="A19" s="10"/>
-      <c r="B19" s="11"/>
-      <c r="C19" s="12" t="s">
-        <v>34</v>
-      </c>
-      <c r="D19" s="12" t="s">
-        <v>32</v>
-      </c>
-      <c r="E19" s="12" t="s">
-        <v>27</v>
-      </c>
-      <c r="F19" s="13">
-        <v>175</v>
-      </c>
-      <c r="G19" s="14">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="20" spans="1:7" x14ac:dyDescent="0.45">
-      <c r="A20" s="10"/>
-      <c r="B20" s="11"/>
-      <c r="C20" s="12" t="s">
-        <v>25</v>
-      </c>
-      <c r="D20" s="12" t="s">
-        <v>30</v>
-      </c>
-      <c r="E20" s="12" t="s">
-        <v>27</v>
-      </c>
-      <c r="F20" s="13">
-        <v>175</v>
-      </c>
-      <c r="G20" s="14">
         <v>1</v>
       </c>
     </row>

</xml_diff>

<commit_message>
rename Pmax to PmaxLink
</commit_message>
<xml_diff>
--- a/data/example/Power_Links.xlsx
+++ b/data/example/Power_Links.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\micha\Desktop\GIT\LEGO-Pyomo\data\example\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{81DD55D1-2383-46E0-BC61-E50F84394C18}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{489CF028-2E74-4241-A9A0-58DFF63E48C1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-98" yWindow="-98" windowWidth="21795" windowHeight="13875" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -152,9 +152,6 @@
     <t>c</t>
   </si>
   <si>
-    <t>pPmax</t>
-  </si>
-  <si>
     <t>ID within database</t>
   </si>
   <si>
@@ -264,6 +261,9 @@
   </si>
   <si>
     <t>Node_9.1</t>
+  </si>
+  <si>
+    <t>pPmaxLink</t>
   </si>
 </sst>
 </file>
@@ -391,10 +391,10 @@
     <xf numFmtId="0" fontId="5" fillId="7" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment indent="1"/>
     </xf>
-    <xf numFmtId="1" fontId="5" fillId="7" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="5" fillId="6" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center"/>
     </xf>
-    <xf numFmtId="164" fontId="5" fillId="6" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="5" fillId="7" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center"/>
     </xf>
   </cellXfs>
@@ -708,7 +708,7 @@
       <pane xSplit="2" ySplit="7" topLeftCell="C8" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight"/>
       <selection pane="bottomLeft"/>
-      <selection pane="bottomRight" activeCell="I6" sqref="I6"/>
+      <selection pane="bottomRight" activeCell="F4" sqref="F4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.1328125" defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
@@ -721,7 +721,7 @@
     <row r="1" spans="1:7" ht="23.25" x14ac:dyDescent="0.7">
       <c r="A1" s="1"/>
       <c r="B1" s="2" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="C1" s="1"/>
       <c r="D1" s="1"/>
@@ -734,7 +734,7 @@
         <v>0</v>
       </c>
       <c r="C2" s="4" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.45">
@@ -757,7 +757,7 @@
         <v>6</v>
       </c>
       <c r="G3" s="5" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
     </row>
     <row r="4" spans="1:7" x14ac:dyDescent="0.45">
@@ -777,91 +777,91 @@
         <v>11</v>
       </c>
       <c r="F4" s="6" t="s">
-        <v>12</v>
+        <v>49</v>
       </c>
       <c r="G4" s="6" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
     </row>
     <row r="5" spans="1:7" ht="45" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A5" s="7"/>
       <c r="B5" s="7" t="s">
+        <v>12</v>
+      </c>
+      <c r="C5" s="7" t="s">
         <v>13</v>
       </c>
-      <c r="C5" s="7" t="s">
+      <c r="D5" s="7" t="s">
         <v>14</v>
       </c>
-      <c r="D5" s="7" t="s">
+      <c r="E5" s="7" t="s">
         <v>15</v>
       </c>
-      <c r="E5" s="7" t="s">
+      <c r="F5" s="7" t="s">
         <v>16</v>
       </c>
-      <c r="F5" s="7" t="s">
-        <v>17</v>
-      </c>
       <c r="G5" s="7" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
     </row>
     <row r="6" spans="1:7" ht="30" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A6" s="8"/>
       <c r="B6" s="8" t="s">
+        <v>17</v>
+      </c>
+      <c r="C6" s="8" t="s">
         <v>18</v>
       </c>
-      <c r="C6" s="8" t="s">
+      <c r="D6" s="8" t="s">
+        <v>18</v>
+      </c>
+      <c r="E6" s="8" t="s">
+        <v>18</v>
+      </c>
+      <c r="F6" s="8" t="s">
+        <v>18</v>
+      </c>
+      <c r="G6" s="8" t="s">
         <v>19</v>
-      </c>
-      <c r="D6" s="8" t="s">
-        <v>19</v>
-      </c>
-      <c r="E6" s="8" t="s">
-        <v>19</v>
-      </c>
-      <c r="F6" s="8" t="s">
-        <v>19</v>
-      </c>
-      <c r="G6" s="8" t="s">
-        <v>20</v>
       </c>
     </row>
     <row r="7" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A7" s="9"/>
       <c r="B7" s="9" t="s">
+        <v>20</v>
+      </c>
+      <c r="C7" s="9" t="s">
         <v>21</v>
       </c>
-      <c r="C7" s="9" t="s">
+      <c r="D7" s="9" t="s">
+        <v>21</v>
+      </c>
+      <c r="E7" s="9" t="s">
         <v>22</v>
       </c>
-      <c r="D7" s="9" t="s">
-        <v>22</v>
-      </c>
-      <c r="E7" s="9" t="s">
+      <c r="F7" s="9" t="s">
         <v>23</v>
       </c>
-      <c r="F7" s="9" t="s">
-        <v>24</v>
-      </c>
       <c r="G7" s="9" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
     </row>
     <row r="8" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A8" s="10"/>
       <c r="B8" s="11"/>
       <c r="C8" s="12" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="D8" s="12" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="E8" s="12" t="s">
-        <v>27</v>
-      </c>
-      <c r="F8" s="13">
-        <v>175</v>
-      </c>
-      <c r="G8" s="14">
+        <v>26</v>
+      </c>
+      <c r="F8" s="14">
+        <v>672.60519999999997</v>
+      </c>
+      <c r="G8" s="13">
         <v>1</v>
       </c>
     </row>
@@ -869,18 +869,18 @@
       <c r="A9" s="10"/>
       <c r="B9" s="11"/>
       <c r="C9" s="12" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="D9" s="12" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="E9" s="12" t="s">
-        <v>27</v>
-      </c>
-      <c r="F9" s="13">
-        <v>175</v>
-      </c>
-      <c r="G9" s="14">
+        <v>26</v>
+      </c>
+      <c r="F9" s="14">
+        <v>313.88240000000002</v>
+      </c>
+      <c r="G9" s="13">
         <v>1</v>
       </c>
     </row>
@@ -888,18 +888,18 @@
       <c r="A10" s="10"/>
       <c r="B10" s="11"/>
       <c r="C10" s="12" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="D10" s="12" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="E10" s="12" t="s">
-        <v>27</v>
-      </c>
-      <c r="F10" s="13">
-        <v>175</v>
-      </c>
-      <c r="G10" s="14">
+        <v>26</v>
+      </c>
+      <c r="F10" s="14">
+        <v>448.40350000000001</v>
+      </c>
+      <c r="G10" s="13">
         <v>1</v>
       </c>
     </row>
@@ -907,18 +907,18 @@
       <c r="A11" s="10"/>
       <c r="B11" s="11"/>
       <c r="C11" s="12" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="D11" s="12" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="E11" s="12" t="s">
-        <v>27</v>
-      </c>
-      <c r="F11" s="13">
-        <v>175</v>
-      </c>
-      <c r="G11" s="14">
+        <v>26</v>
+      </c>
+      <c r="F11" s="14">
+        <v>896.80690000000004</v>
+      </c>
+      <c r="G11" s="13">
         <v>1</v>
       </c>
     </row>
@@ -926,18 +926,18 @@
       <c r="A12" s="10"/>
       <c r="B12" s="11"/>
       <c r="C12" s="12" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="D12" s="12" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="E12" s="12" t="s">
-        <v>27</v>
-      </c>
-      <c r="F12" s="13">
-        <v>175</v>
-      </c>
-      <c r="G12" s="14">
+        <v>26</v>
+      </c>
+      <c r="F12" s="14">
+        <v>1661.2634</v>
+      </c>
+      <c r="G12" s="13">
         <v>1</v>
       </c>
     </row>
@@ -945,18 +945,18 @@
       <c r="A13" s="10"/>
       <c r="B13" s="11"/>
       <c r="C13" s="12" t="s">
+        <v>25</v>
+      </c>
+      <c r="D13" s="12" t="s">
+        <v>45</v>
+      </c>
+      <c r="E13" s="12" t="s">
         <v>26</v>
       </c>
-      <c r="D13" s="12" t="s">
-        <v>46</v>
-      </c>
-      <c r="E13" s="12" t="s">
-        <v>27</v>
-      </c>
-      <c r="F13" s="13">
-        <v>175</v>
-      </c>
-      <c r="G13" s="14">
+      <c r="F13" s="14">
+        <v>2028.3655000000001</v>
+      </c>
+      <c r="G13" s="13">
         <v>1</v>
       </c>
     </row>
@@ -964,18 +964,18 @@
       <c r="A14" s="10"/>
       <c r="B14" s="11"/>
       <c r="C14" s="12" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="D14" s="12" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="E14" s="12" t="s">
-        <v>27</v>
-      </c>
-      <c r="F14" s="13">
-        <v>175</v>
-      </c>
-      <c r="G14" s="14">
+        <v>26</v>
+      </c>
+      <c r="F14" s="14">
+        <v>358.72280000000001</v>
+      </c>
+      <c r="G14" s="13">
         <v>1</v>
       </c>
     </row>
@@ -983,18 +983,18 @@
       <c r="A15" s="10"/>
       <c r="B15" s="11"/>
       <c r="C15" s="12" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="D15" s="12" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="E15" s="12" t="s">
-        <v>27</v>
-      </c>
-      <c r="F15" s="13">
-        <v>175</v>
-      </c>
-      <c r="G15" s="14">
+        <v>26</v>
+      </c>
+      <c r="F15" s="14">
+        <v>2300.5331000000001</v>
+      </c>
+      <c r="G15" s="13">
         <v>1</v>
       </c>
     </row>
@@ -1002,18 +1002,18 @@
       <c r="A16" s="10"/>
       <c r="B16" s="11"/>
       <c r="C16" s="12" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="D16" s="12" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="E16" s="12" t="s">
-        <v>27</v>
-      </c>
-      <c r="F16" s="13">
-        <v>175</v>
-      </c>
-      <c r="G16" s="14">
+        <v>26</v>
+      </c>
+      <c r="F16" s="14">
+        <v>224.20169999999999</v>
+      </c>
+      <c r="G16" s="13">
         <v>1</v>
       </c>
     </row>

</xml_diff>